<commit_message>
E.H.R - Tabs Vs. Tables
</commit_message>
<xml_diff>
--- a/E.H.R.xlsx
+++ b/E.H.R.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="E.H.R" sheetId="1" r:id="rId1"/>
     <sheet name="Tabs Vs. Tables" sheetId="2" r:id="rId2"/>
+    <sheet name="Notes" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -78,12 +79,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="A15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>vasuprasad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maintain as part of E.H.R?</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
   <si>
     <t>E.H.R</t>
   </si>
@@ -103,9 +128,6 @@
     <t>PROBLEM LIST</t>
   </si>
   <si>
-    <t>NOTES</t>
-  </si>
-  <si>
     <t>PHYSICIAN'S ORDERS</t>
   </si>
   <si>
@@ -265,12 +287,6 @@
     <t>patientrelativeproblem</t>
   </si>
   <si>
-    <t>Encounter Details</t>
-  </si>
-  <si>
-    <t>encounter</t>
-  </si>
-  <si>
     <t>labtests</t>
   </si>
   <si>
@@ -295,15 +311,9 @@
     <t>Prescription</t>
   </si>
   <si>
-    <t>presription</t>
-  </si>
-  <si>
     <t>RECOMMENDATIONS</t>
   </si>
   <si>
-    <t>VITALS</t>
-  </si>
-  <si>
     <t>Immunization</t>
   </si>
   <si>
@@ -311,13 +321,64 @@
   </si>
   <si>
     <t>Yet to be designed</t>
+  </si>
+  <si>
+    <t>A Vist can have multiple encounters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encounters with more than one health professional and multiple encounters with the same </t>
+  </si>
+  <si>
+    <t xml:space="preserve">health professionals which take place on the same day and at a single location constitute a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">single visit, except when one of the following conditions exist: (a) after the first </t>
+  </si>
+  <si>
+    <t xml:space="preserve">encounter, the patient suffers illness or injury requiring additional diagnosis or treatment; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(b) the patient has a medical visit and a clinical psychologist or clinical social worker </t>
+  </si>
+  <si>
+    <t>visit</t>
+  </si>
+  <si>
+    <t>Vital Sign Results</t>
+  </si>
+  <si>
+    <t>vitalsignobservation</t>
+  </si>
+  <si>
+    <t>prescription</t>
+  </si>
+  <si>
+    <t>ORDERS &amp; OBSERATIONS</t>
+  </si>
+  <si>
+    <t>CARE PLAN</t>
+  </si>
+  <si>
+    <t>VISITS &amp; NOTES</t>
+  </si>
+  <si>
+    <t>Visit Details</t>
+  </si>
+  <si>
+    <t>VITAL SIGNS</t>
+  </si>
+  <si>
+    <t>NIVARC</t>
+  </si>
+  <si>
+    <t>visits &amp; encounters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,8 +448,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="64"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,8 +504,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -468,11 +571,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -492,9 +676,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,6 +685,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -513,22 +716,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -829,229 +1029,229 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="C16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1062,39 +1262,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.42578125" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="11" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="26"/>
+      <c r="M1" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="25"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1105,171 +1318,347 @@
         <v>5</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>64</v>
+      <c r="E8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="G10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="5"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="6" t="s">
+      <c r="I12" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="5" t="s">
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="C18" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>75</v>
-      </c>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="24">
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
     <mergeCell ref="C1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="84.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>